<commit_message>
fix t49 data upload
</commit_message>
<xml_diff>
--- a/warehouse/utils/data/20240826_additional_containers/data.xlsx
+++ b/warehouse/utils/data/20240826_additional_containers/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>container_number</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t xml:space="preserve">SEGU4133320 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UETU5190944 </t>
   </si>
   <si>
     <t xml:space="preserve">FFAU2821522 </t>
@@ -387,19 +384,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -435,12 +426,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -748,628 +736,623 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A123"/>
+  <dimension ref="A1:A122"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="17.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" hidden="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" hidden="1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25" hidden="1">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25" hidden="1">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25" hidden="1">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25" hidden="1">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25" hidden="1">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21.75">
-      <c r="A8" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25" hidden="1">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" hidden="1">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" hidden="1">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25" hidden="1">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" hidden="1">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25" hidden="1">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25" hidden="1">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25" hidden="1">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25" hidden="1">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" hidden="1">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" hidden="1">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25" hidden="1">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25" hidden="1">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25" hidden="1">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25" hidden="1">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25" hidden="1">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" hidden="1">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" hidden="1">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25" hidden="1">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" hidden="1">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25" hidden="1">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" hidden="1">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" hidden="1">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" hidden="1">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" hidden="1">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
-      <c r="A33" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25" hidden="1">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
-      <c r="A34" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25" hidden="1">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
-      <c r="A35" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" hidden="1">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
-      <c r="A36" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" hidden="1">
+      <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
-      <c r="A37" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" hidden="1">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
-      <c r="A38" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" hidden="1">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
-      <c r="A39" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25" hidden="1">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
-      <c r="A40" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" hidden="1">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
-      <c r="A41" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" hidden="1">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
-      <c r="A42" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" hidden="1">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
-      <c r="A43" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25" hidden="1">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
-      <c r="A44" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" hidden="1">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
-      <c r="A45" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25" hidden="1">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
-      <c r="A46" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" hidden="1">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
-      <c r="A47" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25" hidden="1">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
-      <c r="A48" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25" hidden="1">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
-      <c r="A49" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" hidden="1">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
-      <c r="A50" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25" hidden="1">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
-      <c r="A51" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25" hidden="1">
+      <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
-      <c r="A52" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25" hidden="1">
+      <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
-      <c r="A53" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25" hidden="1">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
-      <c r="A54" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25" hidden="1">
+      <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
-      <c r="A55" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25" hidden="1">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
-      <c r="A56" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25" hidden="1">
+      <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
-      <c r="A57" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25" hidden="1">
+      <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
-      <c r="A58" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25" hidden="1">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
-      <c r="A59" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25" hidden="1">
+      <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
-      <c r="A60" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25" hidden="1">
+      <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
-      <c r="A61" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25" hidden="1">
+      <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
-      <c r="A62" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25" hidden="1">
+      <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
-      <c r="A63" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25" hidden="1">
+      <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
-      <c r="A64" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25" hidden="1">
+      <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
-      <c r="A65" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25" hidden="1">
+      <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
-      <c r="A66" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25" hidden="1">
+      <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
-      <c r="A67" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25" hidden="1">
+      <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
-      <c r="A68" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25" hidden="1">
+      <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
-      <c r="A69" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25" hidden="1">
+      <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
-      <c r="A70" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25" hidden="1">
+      <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
-      <c r="A71" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25" hidden="1">
+      <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
-      <c r="A72" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25" hidden="1">
+      <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
-      <c r="A73" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25" hidden="1">
+      <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
-      <c r="A74" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25" hidden="1">
+      <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
-      <c r="A75" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25" hidden="1">
+      <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
-      <c r="A76" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25" hidden="1">
+      <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
-      <c r="A77" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25" hidden="1">
+      <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
-      <c r="A78" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25" hidden="1">
+      <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
-      <c r="A79" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25" hidden="1">
+      <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
-      <c r="A80" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25" hidden="1">
+      <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
-      <c r="A81" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25" hidden="1">
+      <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
-      <c r="A82" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25" hidden="1">
+      <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
-      <c r="A83" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25" hidden="1">
+      <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
-      <c r="A84" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25" hidden="1">
+      <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
-      <c r="A85" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25" hidden="1">
+      <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
-      <c r="A86" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25" hidden="1">
+      <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
-      <c r="A87" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25" hidden="1">
+      <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
-      <c r="A88" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25" hidden="1">
+      <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
-      <c r="A89" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25" hidden="1">
+      <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
-      <c r="A90" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25" hidden="1">
+      <c r="A90" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25" hidden="1">
+      <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
-      <c r="A91" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
-      <c r="A92" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25" hidden="1">
+      <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
-      <c r="A93" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25" hidden="1">
+      <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
-      <c r="A94" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25" hidden="1">
+      <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
-      <c r="A95" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25" hidden="1">
+      <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
-      <c r="A96" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25" hidden="1">
+      <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
-      <c r="A97" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25" hidden="1">
+      <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
-      <c r="A98" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25" hidden="1">
+      <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
-      <c r="A99" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25" hidden="1">
+      <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
-      <c r="A100" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25" hidden="1">
+      <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
-      <c r="A101" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25" hidden="1">
+      <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
-      <c r="A102" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25" hidden="1">
+      <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
-      <c r="A103" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25" hidden="1">
+      <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
-      <c r="A104" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25" hidden="1">
+      <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
-      <c r="A105" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25" hidden="1">
+      <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
-      <c r="A106" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25" hidden="1">
+      <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
-      <c r="A107" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25" hidden="1">
+      <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
-      <c r="A108" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25" hidden="1">
+      <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
-      <c r="A109" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25" hidden="1">
+      <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
-      <c r="A110" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25" hidden="1">
+      <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
-      <c r="A111" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25" hidden="1">
+      <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25">
-      <c r="A112" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25" hidden="1">
+      <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25">
-      <c r="A113" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25" hidden="1">
+      <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25">
-      <c r="A114" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25" hidden="1">
+      <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25">
-      <c r="A115" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25" hidden="1">
+      <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25">
-      <c r="A116" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25" hidden="1">
+      <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25">
-      <c r="A117" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25" hidden="1">
+      <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25">
-      <c r="A118" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25" hidden="1">
+      <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25">
-      <c r="A119" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25" hidden="1">
+      <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25">
-      <c r="A120" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25" hidden="1">
+      <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25">
-      <c r="A121" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25" hidden="1">
+      <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25">
-      <c r="A122" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25" hidden="1">
+      <c r="A122" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="17.25">
-      <c r="A123" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>